<commit_message>
Add equipment and lab reservation features with CRUD operations, update routing, and enhance UI with new data handling and navigation improvements
</commit_message>
<xml_diff>
--- a/public/assets/file/labReservation/example/example-template.xlsx
+++ b/public/assets/file/labReservation/example/example-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goodb\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Storage\prj\LabConnect\labConnect\public\assets\file\labReservation\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{99EA5766-EB22-4626-B448-8567295CF7B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83616FFE-B843-451B-A6C3-50DDC39847E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9420" xr2:uid="{A3354791-E2B1-4E03-99FB-F358E8C18B31}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A3354791-E2B1-4E03-99FB-F358E8C18B31}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>No</t>
   </si>
   <si>
     <t>Nim</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Andi</t>
+  </si>
+  <si>
+    <t>Eka</t>
   </si>
 </sst>
 </file>
@@ -413,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B4A085-08EE-45FD-846B-6D3A7C837CA7}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -424,28 +433,37 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>119703003</v>
       </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>119703004</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>